<commit_message>
EPBDS: added tests for base implementations of mapping aware custom converters and field mapping conditions.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/thread/MappingParamsAwareFieldMappingConditionThreadSafetyTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/thread/MappingParamsAwareFieldMappingConditionThreadSafetyTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>classA</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>mapField</t>
+  </si>
+  <si>
+    <t>Wildcard</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C7:L18"/>
+  <dimension ref="C7:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -507,13 +510,13 @@
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:12">
+    <row r="7" spans="3:7">
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="3:12">
+    <row r="8" spans="3:7">
       <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
@@ -521,25 +524,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:12">
+    <row r="9" spans="3:7">
       <c r="C9" s="7"/>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="3:12">
+    <row r="10" spans="3:7">
       <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="3:12">
+    <row r="11" spans="3:7">
       <c r="C11" s="7"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="3:12">
+    <row r="15" spans="3:7">
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
@@ -547,11 +550,8 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="L15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12">
+    </row>
+    <row r="16" spans="3:7">
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,11 +567,8 @@
       <c r="G16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" ht="30">
+    </row>
+    <row r="17" spans="3:7" ht="30">
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -587,11 +584,8 @@
       <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12">
+    </row>
+    <row r="18" spans="3:7">
       <c r="C18" t="s">
         <v>17</v>
       </c>
@@ -607,7 +601,24 @@
       <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="L18" t="b">
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>